<commit_message>
adding spike in fastq file for exp 28 and 29, updated date error in exp 28 library file
</commit_message>
<xml_diff>
--- a/library/Library_J.PLAGGENBERG_10.05.20.xlsx
+++ b/library/Library_J.PLAGGENBERG_10.05.20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicaplaggenberg/Documents/rnaseq-database/library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC4422E1-2686-CA44-82BA-219637EF6F6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3550FF-52D4-3E4A-8481-43DCC5AAE129}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="620" windowWidth="15920" windowHeight="19700" xr2:uid="{AD7DC79B-FBCE-7148-8D6C-6199D187BA8B}"/>
+    <workbookView xWindow="500" yWindow="600" windowWidth="15920" windowHeight="19700" xr2:uid="{AD7DC79B-FBCE-7148-8D6C-6199D187BA8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -170,7 +170,7 @@
     <t>10.01.20</t>
   </si>
   <si>
-    <t>10.05.2020</t>
+    <t>10.05.20</t>
   </si>
 </sst>
 </file>
@@ -525,7 +525,7 @@
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>